<commit_message>
changes for planning integration with flask
</commit_message>
<xml_diff>
--- a/data/student_data.xlsx
+++ b/data/student_data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="99">
   <si>
     <t>Student Name</t>
   </si>
@@ -200,9 +200,6 @@
     <t>Assign duration to actions.</t>
   </si>
   <si>
-    <t>Prerequisites</t>
-  </si>
-  <si>
     <t>FreeCell</t>
   </si>
   <si>
@@ -212,9 +209,6 @@
     <t>Depot</t>
   </si>
   <si>
-    <t>T5, T6</t>
-  </si>
-  <si>
     <t>This domain was devised in order to see what would happen if two previously well-researched domains were joined together. These were the logistics and blocks domains. They are combined to form a domain in which trucks can transport crates around and then the crates must be stacked onto pallets at their destinations. The stacking is achieved using hoists, so the stacking problem is like a blocks-world problem with hands. Trucks can behave like "tables", since the pallets on which crates are stacked are limited.</t>
   </si>
   <si>
@@ -239,9 +233,6 @@
     <t>Satellite</t>
   </si>
   <si>
-    <t>T9, T10</t>
-  </si>
-  <si>
     <t>The first of the domains inspired by space-applications. It involves planning and scheduling a collection of observation tasks between multiple satellites, each equipped in slightly different ways.</t>
   </si>
   <si>
@@ -263,9 +254,6 @@
     <t>equality</t>
   </si>
   <si>
-    <t>functions</t>
-  </si>
-  <si>
     <t>adl</t>
   </si>
   <si>
@@ -300,6 +288,36 @@
   </si>
   <si>
     <t>Learn how to write definition of start and goal states. Formatting of problem.pddl</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>functions, action-costs</t>
+  </si>
+  <si>
+    <t>adl, conditional-effects</t>
+  </si>
+  <si>
+    <t>adl, domain-axioms, conditional-effects</t>
+  </si>
+  <si>
+    <t>strips, propositions, operators, states, action-costs, typing</t>
+  </si>
+  <si>
+    <t>functions, negative-conditions, equality</t>
   </si>
 </sst>
 </file>
@@ -684,7 +702,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -727,13 +745,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
-        <v>1</v>
+      <c r="A2" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
-        <v>2</v>
+      <c r="A3" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -752,8 +770,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
-        <v>3</v>
+      <c r="A4" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
@@ -772,8 +790,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
-        <v>4</v>
+      <c r="A5" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
@@ -786,8 +804,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
-        <v>5</v>
+      <c r="A6" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -800,7 +818,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -824,7 +842,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>17</v>
@@ -838,7 +856,7 @@
         <v>31</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>48</v>
@@ -855,7 +873,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>49</v>
@@ -872,10 +890,10 @@
         <v>19</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -889,10 +907,10 @@
         <v>19</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
@@ -906,7 +924,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>50</v>
@@ -923,7 +941,7 @@
         <v>47</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>51</v>
@@ -940,7 +958,7 @@
         <v>47</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>52</v>
@@ -957,7 +975,7 @@
         <v>20</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>53</v>
@@ -974,7 +992,7 @@
         <v>23</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>54</v>
@@ -991,7 +1009,7 @@
         <v>46</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>55</v>
@@ -1008,7 +1026,7 @@
         <v>45</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>56</v>
@@ -1025,7 +1043,7 @@
         <v>44</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>57</v>
@@ -1042,7 +1060,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>58</v>
@@ -1056,127 +1074,162 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13A56AB-9175-4CF8-8F7C-C9D141F14755}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="18.06640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1328125" customWidth="1"/>
-    <col min="4" max="4" width="45.265625" customWidth="1"/>
-    <col min="5" max="5" width="72.53125" customWidth="1"/>
+    <col min="3" max="3" width="45.265625" customWidth="1"/>
+    <col min="4" max="4" width="72.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="78.75" x14ac:dyDescent="0.45">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="78.75" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="39.4" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="39.4" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="52.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="52.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="39.4" x14ac:dyDescent="0.45">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="39.4" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C24" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>